<commit_message>
Update a SI figure and Table S5
</commit_message>
<xml_diff>
--- a/output/FigSourceData/MainTab_connection.xlsx
+++ b/output/FigSourceData/MainTab_connection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GCAM\Archive\paper-LandBasedCDR-DisplayItems\output\FigSourceData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FED8A1D-DF57-4584-9337-9070B1E55BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FCF1E3-359E-406D-8607-5B5846D84EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="32281" windowHeight="17656" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31943" yWindow="2830" windowWidth="24267" windowHeight="14650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MainTab_connection" sheetId="1" r:id="rId1"/>
@@ -380,10 +380,6 @@
     <t>Variable &amp; Metric</t>
   </si>
   <si>
-    <t xml:space="preserve">Land use change
-(Mha) </t>
-  </si>
-  <si>
     <r>
       <t>Effective land carbon density
 (tCO</t>
@@ -416,31 +412,6 @@
   </si>
   <si>
     <t>LULUCF vs. Forest &amp; Other natural</t>
-  </si>
-  <si>
-    <r>
-      <t>Land mitigation intensity 
-(tCO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> / ha /yr)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -498,6 +469,35 @@
       </rPr>
       <t xml:space="preserve"> / yr)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>Land carbon removal intensity 
+(tCO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> / ha /yr)</t>
+    </r>
+  </si>
+  <si>
+    <t>Land carbon removal intensity 
+(tCO2 / ha /yr)</t>
   </si>
 </sst>
 </file>
@@ -1300,12 +1300,6 @@
     <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="39" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1315,7 +1309,40 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="40" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1331,33 +1358,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4446,59 +4446,59 @@
       <c r="C4" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="73" t="s">
+      <c r="D4" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73" t="s">
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73" t="s">
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73" t="s">
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
       <c r="S4" s="51"/>
       <c r="T4" s="51"/>
       <c r="U4" s="51"/>
-      <c r="V4" s="78" t="s">
+      <c r="V4" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="W4" s="78"/>
-      <c r="X4" s="73" t="s">
+      <c r="W4" s="87"/>
+      <c r="X4" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="73" t="s">
+      <c r="Y4" s="71"/>
+      <c r="Z4" s="71"/>
+      <c r="AA4" s="71"/>
+      <c r="AB4" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="AC4" s="73"/>
-      <c r="AD4" s="73"/>
-      <c r="AE4" s="73" t="s">
+      <c r="AC4" s="71"/>
+      <c r="AD4" s="71"/>
+      <c r="AE4" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="AF4" s="73"/>
-      <c r="AG4" s="73"/>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="73" t="s">
+      <c r="AF4" s="71"/>
+      <c r="AG4" s="71"/>
+      <c r="AH4" s="71"/>
+      <c r="AI4" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="AJ4" s="73"/>
-      <c r="AK4" s="73"/>
-      <c r="AL4" s="73"/>
+      <c r="AJ4" s="71"/>
+      <c r="AK4" s="71"/>
+      <c r="AL4" s="71"/>
     </row>
     <row r="5" spans="2:38" ht="54.5" x14ac:dyDescent="0.2">
       <c r="B5" s="4"/>
@@ -4551,8 +4551,8 @@
       <c r="S5" s="52"/>
       <c r="T5" s="52"/>
       <c r="U5" s="52"/>
-      <c r="V5" s="79"/>
-      <c r="W5" s="79"/>
+      <c r="V5" s="88"/>
+      <c r="W5" s="88"/>
       <c r="X5" s="5" t="s">
         <v>53</v>
       </c>
@@ -4600,43 +4600,43 @@
       </c>
     </row>
     <row r="6" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="72" t="s">
         <v>57</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="88">
+      <c r="D6" s="75">
         <f>1150/81</f>
         <v>14.197530864197532</v>
       </c>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88">
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75">
         <f>1150/81</f>
         <v>14.197530864197532</v>
       </c>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88">
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75">
         <f>1150/81</f>
         <v>14.197530864197532</v>
       </c>
-      <c r="L6" s="88"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88">
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="75">
         <f>500/81</f>
         <v>6.1728395061728394</v>
       </c>
-      <c r="P6" s="88"/>
-      <c r="Q6" s="88"/>
-      <c r="R6" s="88"/>
+      <c r="P6" s="75"/>
+      <c r="Q6" s="75"/>
+      <c r="R6" s="75"/>
       <c r="S6" s="53"/>
       <c r="T6" s="53"/>
       <c r="U6" s="53"/>
-      <c r="V6" s="80" t="s">
+      <c r="V6" s="72" t="s">
         <v>57</v>
       </c>
       <c r="W6" s="6" t="s">
@@ -4644,7 +4644,7 @@
       </c>
     </row>
     <row r="7" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B7" s="81"/>
+      <c r="B7" s="73"/>
       <c r="C7" s="8" t="s">
         <v>59</v>
       </c>
@@ -4711,7 +4711,7 @@
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
       <c r="U7" s="9"/>
-      <c r="V7" s="81"/>
+      <c r="V7" s="73"/>
       <c r="W7" s="8" t="s">
         <v>59</v>
       </c>
@@ -4777,7 +4777,7 @@
       </c>
     </row>
     <row r="8" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B8" s="81"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="8" t="s">
         <v>60</v>
       </c>
@@ -4844,7 +4844,7 @@
       <c r="S8" s="9"/>
       <c r="T8" s="9"/>
       <c r="U8" s="9"/>
-      <c r="V8" s="81"/>
+      <c r="V8" s="73"/>
       <c r="W8" s="8" t="s">
         <v>60</v>
       </c>
@@ -4910,7 +4910,7 @@
       </c>
     </row>
     <row r="9" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B9" s="81"/>
+      <c r="B9" s="73"/>
       <c r="C9" s="8" t="s">
         <v>61</v>
       </c>
@@ -4977,7 +4977,7 @@
       <c r="S9" s="9"/>
       <c r="T9" s="9"/>
       <c r="U9" s="9"/>
-      <c r="V9" s="81"/>
+      <c r="V9" s="73"/>
       <c r="W9" s="8" t="s">
         <v>61</v>
       </c>
@@ -5043,7 +5043,7 @@
       </c>
     </row>
     <row r="10" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B10" s="82"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="15" t="s">
         <v>23</v>
       </c>
@@ -5110,7 +5110,7 @@
       <c r="S10" s="16"/>
       <c r="T10" s="16"/>
       <c r="U10" s="16"/>
-      <c r="V10" s="82"/>
+      <c r="V10" s="74"/>
       <c r="W10" s="15" t="s">
         <v>23</v>
       </c>
@@ -5215,7 +5215,7 @@
       <c r="AL11" s="30"/>
     </row>
     <row r="12" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="81" t="s">
         <v>63</v>
       </c>
       <c r="C12" s="36" t="s">
@@ -5284,7 +5284,7 @@
       <c r="S12" s="17"/>
       <c r="T12" s="17"/>
       <c r="U12" s="17"/>
-      <c r="V12" s="83" t="s">
+      <c r="V12" s="81" t="s">
         <v>63</v>
       </c>
       <c r="W12" s="36" t="s">
@@ -5352,7 +5352,7 @@
       </c>
     </row>
     <row r="13" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B13" s="84"/>
+      <c r="B13" s="82"/>
       <c r="C13" s="36" t="s">
         <v>64</v>
       </c>
@@ -5419,7 +5419,7 @@
       <c r="S13" s="17"/>
       <c r="T13" s="17"/>
       <c r="U13" s="17"/>
-      <c r="V13" s="84"/>
+      <c r="V13" s="82"/>
       <c r="W13" s="36" t="s">
         <v>64</v>
       </c>
@@ -5485,7 +5485,7 @@
       </c>
     </row>
     <row r="14" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B14" s="84"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="37" t="s">
         <v>28</v>
       </c>
@@ -5552,7 +5552,7 @@
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
-      <c r="V14" s="84"/>
+      <c r="V14" s="82"/>
       <c r="W14" s="37" t="s">
         <v>28</v>
       </c>
@@ -5618,7 +5618,7 @@
       </c>
     </row>
     <row r="15" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B15" s="84"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="37" t="s">
         <v>65</v>
       </c>
@@ -5685,7 +5685,7 @@
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
-      <c r="V15" s="84"/>
+      <c r="V15" s="82"/>
       <c r="W15" s="37" t="s">
         <v>65</v>
       </c>
@@ -5751,7 +5751,7 @@
       </c>
     </row>
     <row r="16" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B16" s="84"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="37" t="s">
         <v>30</v>
       </c>
@@ -5818,7 +5818,7 @@
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
-      <c r="V16" s="84"/>
+      <c r="V16" s="82"/>
       <c r="W16" s="37" t="s">
         <v>30</v>
       </c>
@@ -5884,7 +5884,7 @@
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B17" s="84"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="37" t="s">
         <v>31</v>
       </c>
@@ -5951,7 +5951,7 @@
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
       <c r="U17" s="10"/>
-      <c r="V17" s="84"/>
+      <c r="V17" s="82"/>
       <c r="W17" s="37" t="s">
         <v>31</v>
       </c>
@@ -6017,7 +6017,7 @@
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B18" s="84"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="37" t="s">
         <v>32</v>
       </c>
@@ -6084,7 +6084,7 @@
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
-      <c r="V18" s="84"/>
+      <c r="V18" s="82"/>
       <c r="W18" s="37" t="s">
         <v>32</v>
       </c>
@@ -6150,7 +6150,7 @@
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B19" s="85"/>
+      <c r="B19" s="83"/>
       <c r="C19" s="36" t="s">
         <v>26</v>
       </c>
@@ -6217,7 +6217,7 @@
       <c r="S19" s="17"/>
       <c r="T19" s="17"/>
       <c r="U19" s="17"/>
-      <c r="V19" s="85"/>
+      <c r="V19" s="83"/>
       <c r="W19" s="36" t="s">
         <v>26</v>
       </c>
@@ -6323,7 +6323,7 @@
       <c r="AL20" s="30"/>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B21" s="86" t="s">
+      <c r="B21" s="76" t="s">
         <v>83</v>
       </c>
       <c r="C21" s="38" t="s">
@@ -6392,7 +6392,7 @@
       <c r="S21" s="11"/>
       <c r="T21" s="11"/>
       <c r="U21" s="11"/>
-      <c r="V21" s="86" t="s">
+      <c r="V21" s="76" t="s">
         <v>83</v>
       </c>
       <c r="W21" s="38" t="s">
@@ -6460,7 +6460,7 @@
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B22" s="87"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="39" t="s">
         <v>28</v>
       </c>
@@ -6527,7 +6527,7 @@
       <c r="S22" s="11"/>
       <c r="T22" s="11"/>
       <c r="U22" s="11"/>
-      <c r="V22" s="87"/>
+      <c r="V22" s="77"/>
       <c r="W22" s="39" t="s">
         <v>28</v>
       </c>
@@ -6593,7 +6593,7 @@
       </c>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B23" s="87"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="39" t="s">
         <v>65</v>
       </c>
@@ -6660,7 +6660,7 @@
       <c r="S23" s="11"/>
       <c r="T23" s="11"/>
       <c r="U23" s="11"/>
-      <c r="V23" s="87"/>
+      <c r="V23" s="77"/>
       <c r="W23" s="39" t="s">
         <v>65</v>
       </c>
@@ -6726,7 +6726,7 @@
       </c>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B24" s="87"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="39" t="s">
         <v>66</v>
       </c>
@@ -6793,7 +6793,7 @@
       <c r="S24" s="11"/>
       <c r="T24" s="11"/>
       <c r="U24" s="11"/>
-      <c r="V24" s="87"/>
+      <c r="V24" s="77"/>
       <c r="W24" s="39" t="s">
         <v>66</v>
       </c>
@@ -6859,7 +6859,7 @@
       </c>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B25" s="87"/>
+      <c r="B25" s="77"/>
       <c r="C25" s="39" t="s">
         <v>34</v>
       </c>
@@ -6926,7 +6926,7 @@
       <c r="S25" s="11"/>
       <c r="T25" s="11"/>
       <c r="U25" s="11"/>
-      <c r="V25" s="87"/>
+      <c r="V25" s="77"/>
       <c r="W25" s="39" t="s">
         <v>34</v>
       </c>
@@ -6992,7 +6992,7 @@
       </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B26" s="86"/>
+      <c r="B26" s="76"/>
       <c r="C26" s="38" t="s">
         <v>67</v>
       </c>
@@ -7059,7 +7059,7 @@
       <c r="S26" s="11"/>
       <c r="T26" s="11"/>
       <c r="U26" s="11"/>
-      <c r="V26" s="86"/>
+      <c r="V26" s="76"/>
       <c r="W26" s="38" t="s">
         <v>67</v>
       </c>
@@ -7164,7 +7164,7 @@
       <c r="AL27" s="30"/>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B28" s="74" t="s">
+      <c r="B28" s="78" t="s">
         <v>68</v>
       </c>
       <c r="C28" s="19" t="s">
@@ -7233,7 +7233,7 @@
       <c r="S28" s="20"/>
       <c r="T28" s="20"/>
       <c r="U28" s="20"/>
-      <c r="V28" s="74" t="s">
+      <c r="V28" s="78" t="s">
         <v>68</v>
       </c>
       <c r="W28" s="19" t="s">
@@ -7301,7 +7301,7 @@
       </c>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B29" s="74"/>
+      <c r="B29" s="78"/>
       <c r="C29" s="19" t="s">
         <v>44</v>
       </c>
@@ -7368,7 +7368,7 @@
       <c r="S29" s="20"/>
       <c r="T29" s="20"/>
       <c r="U29" s="20"/>
-      <c r="V29" s="74"/>
+      <c r="V29" s="78"/>
       <c r="W29" s="19" t="s">
         <v>44</v>
       </c>
@@ -7434,7 +7434,7 @@
       </c>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B30" s="74"/>
+      <c r="B30" s="78"/>
       <c r="C30" s="19" t="s">
         <v>45</v>
       </c>
@@ -7501,7 +7501,7 @@
       <c r="S30" s="20"/>
       <c r="T30" s="20"/>
       <c r="U30" s="20"/>
-      <c r="V30" s="74"/>
+      <c r="V30" s="78"/>
       <c r="W30" s="19" t="s">
         <v>45</v>
       </c>
@@ -7567,7 +7567,7 @@
       </c>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B31" s="74"/>
+      <c r="B31" s="78"/>
       <c r="C31" s="19" t="s">
         <v>69</v>
       </c>
@@ -7634,7 +7634,7 @@
       <c r="S31" s="20"/>
       <c r="T31" s="20"/>
       <c r="U31" s="20"/>
-      <c r="V31" s="74"/>
+      <c r="V31" s="78"/>
       <c r="W31" s="19" t="s">
         <v>69</v>
       </c>
@@ -7700,7 +7700,7 @@
       </c>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="B32" s="74"/>
+      <c r="B32" s="78"/>
       <c r="C32" s="19" t="s">
         <v>47</v>
       </c>
@@ -7767,7 +7767,7 @@
       <c r="S32" s="20"/>
       <c r="T32" s="20"/>
       <c r="U32" s="20"/>
-      <c r="V32" s="74"/>
+      <c r="V32" s="78"/>
       <c r="W32" s="19" t="s">
         <v>47</v>
       </c>
@@ -7833,7 +7833,7 @@
       </c>
     </row>
     <row r="33" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B33" s="74"/>
+      <c r="B33" s="78"/>
       <c r="C33" s="19" t="s">
         <v>40</v>
       </c>
@@ -7900,7 +7900,7 @@
       <c r="S33" s="20"/>
       <c r="T33" s="20"/>
       <c r="U33" s="20"/>
-      <c r="V33" s="74"/>
+      <c r="V33" s="78"/>
       <c r="W33" s="19" t="s">
         <v>40</v>
       </c>
@@ -7966,7 +7966,7 @@
       </c>
     </row>
     <row r="34" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B34" s="74"/>
+      <c r="B34" s="78"/>
       <c r="C34" s="19" t="s">
         <v>41</v>
       </c>
@@ -8033,7 +8033,7 @@
       <c r="S34" s="20"/>
       <c r="T34" s="20"/>
       <c r="U34" s="20"/>
-      <c r="V34" s="74"/>
+      <c r="V34" s="78"/>
       <c r="W34" s="19" t="s">
         <v>41</v>
       </c>
@@ -8099,7 +8099,7 @@
       </c>
     </row>
     <row r="35" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B35" s="74"/>
+      <c r="B35" s="78"/>
       <c r="C35" s="19" t="s">
         <v>42</v>
       </c>
@@ -8166,7 +8166,7 @@
       <c r="S35" s="20"/>
       <c r="T35" s="20"/>
       <c r="U35" s="20"/>
-      <c r="V35" s="74"/>
+      <c r="V35" s="78"/>
       <c r="W35" s="19" t="s">
         <v>42</v>
       </c>
@@ -8271,7 +8271,7 @@
       <c r="AL36" s="30"/>
     </row>
     <row r="37" spans="2:38" ht="12.55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="75" t="s">
+      <c r="B37" s="84" t="s">
         <v>84</v>
       </c>
       <c r="C37" s="40" t="s">
@@ -8340,7 +8340,7 @@
       <c r="S37" s="26"/>
       <c r="T37" s="26"/>
       <c r="U37" s="26"/>
-      <c r="V37" s="75" t="s">
+      <c r="V37" s="84" t="s">
         <v>84</v>
       </c>
       <c r="W37" s="40" t="s">
@@ -8408,7 +8408,7 @@
       </c>
     </row>
     <row r="38" spans="2:38" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="76"/>
+      <c r="B38" s="85"/>
       <c r="C38" s="41" t="s">
         <v>42</v>
       </c>
@@ -8475,7 +8475,7 @@
       <c r="S38" s="27"/>
       <c r="T38" s="27"/>
       <c r="U38" s="27"/>
-      <c r="V38" s="76"/>
+      <c r="V38" s="85"/>
       <c r="W38" s="41" t="s">
         <v>42</v>
       </c>
@@ -8541,7 +8541,7 @@
       </c>
     </row>
     <row r="39" spans="2:38" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="76"/>
+      <c r="B39" s="85"/>
       <c r="C39" s="42" t="s">
         <v>81</v>
       </c>
@@ -8608,7 +8608,7 @@
       <c r="S39" s="28"/>
       <c r="T39" s="28"/>
       <c r="U39" s="28"/>
-      <c r="V39" s="76"/>
+      <c r="V39" s="85"/>
       <c r="W39" s="42" t="s">
         <v>81</v>
       </c>
@@ -8674,7 +8674,7 @@
       </c>
     </row>
     <row r="40" spans="2:38" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="75" t="s">
+      <c r="B40" s="84" t="s">
         <v>86</v>
       </c>
       <c r="C40" s="40" t="s">
@@ -8743,7 +8743,7 @@
       <c r="S40" s="26"/>
       <c r="T40" s="26"/>
       <c r="U40" s="26"/>
-      <c r="V40" s="75" t="s">
+      <c r="V40" s="84" t="s">
         <v>86</v>
       </c>
       <c r="W40" s="40" t="s">
@@ -8811,7 +8811,7 @@
       </c>
     </row>
     <row r="41" spans="2:38" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="76"/>
+      <c r="B41" s="85"/>
       <c r="C41" s="41" t="s">
         <v>42</v>
       </c>
@@ -8878,7 +8878,7 @@
       <c r="S41" s="27"/>
       <c r="T41" s="27"/>
       <c r="U41" s="27"/>
-      <c r="V41" s="76"/>
+      <c r="V41" s="85"/>
       <c r="W41" s="41" t="s">
         <v>42</v>
       </c>
@@ -8944,7 +8944,7 @@
       </c>
     </row>
     <row r="42" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B42" s="77"/>
+      <c r="B42" s="86"/>
       <c r="C42" s="42" t="s">
         <v>81</v>
       </c>
@@ -9011,7 +9011,7 @@
       <c r="S42" s="28"/>
       <c r="T42" s="28"/>
       <c r="U42" s="28"/>
-      <c r="V42" s="77"/>
+      <c r="V42" s="86"/>
       <c r="W42" s="42" t="s">
         <v>81</v>
       </c>
@@ -9116,7 +9116,7 @@
       <c r="AL43" s="32"/>
     </row>
     <row r="44" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B44" s="69" t="s">
+      <c r="B44" s="79" t="s">
         <v>85</v>
       </c>
       <c r="C44" s="44" t="s">
@@ -9185,7 +9185,7 @@
       <c r="S44" s="33"/>
       <c r="T44" s="33"/>
       <c r="U44" s="33"/>
-      <c r="V44" s="69" t="s">
+      <c r="V44" s="79" t="s">
         <v>85</v>
       </c>
       <c r="W44" s="44" t="s">
@@ -9253,7 +9253,7 @@
       </c>
     </row>
     <row r="45" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B45" s="70"/>
+      <c r="B45" s="80"/>
       <c r="C45" s="22" t="s">
         <v>59</v>
       </c>
@@ -9320,7 +9320,7 @@
       <c r="S45" s="21"/>
       <c r="T45" s="21"/>
       <c r="U45" s="21"/>
-      <c r="V45" s="70"/>
+      <c r="V45" s="80"/>
       <c r="W45" s="22" t="s">
         <v>59</v>
       </c>
@@ -9386,7 +9386,7 @@
       </c>
     </row>
     <row r="46" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B46" s="70"/>
+      <c r="B46" s="80"/>
       <c r="C46" s="23" t="s">
         <v>60</v>
       </c>
@@ -9453,7 +9453,7 @@
       <c r="S46" s="21"/>
       <c r="T46" s="21"/>
       <c r="U46" s="21"/>
-      <c r="V46" s="70"/>
+      <c r="V46" s="80"/>
       <c r="W46" s="23" t="s">
         <v>60</v>
       </c>
@@ -9519,7 +9519,7 @@
       </c>
     </row>
     <row r="47" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B47" s="70"/>
+      <c r="B47" s="80"/>
       <c r="C47" s="23" t="s">
         <v>71</v>
       </c>
@@ -9586,7 +9586,7 @@
       <c r="S47" s="21"/>
       <c r="T47" s="21"/>
       <c r="U47" s="21"/>
-      <c r="V47" s="70"/>
+      <c r="V47" s="80"/>
       <c r="W47" s="23" t="s">
         <v>71</v>
       </c>
@@ -9652,7 +9652,7 @@
       </c>
     </row>
     <row r="48" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B48" s="70"/>
+      <c r="B48" s="80"/>
       <c r="C48" s="22" t="s">
         <v>72</v>
       </c>
@@ -9719,7 +9719,7 @@
       <c r="S48" s="21"/>
       <c r="T48" s="21"/>
       <c r="U48" s="21"/>
-      <c r="V48" s="70"/>
+      <c r="V48" s="80"/>
       <c r="W48" s="22" t="s">
         <v>72</v>
       </c>
@@ -9785,7 +9785,7 @@
       </c>
     </row>
     <row r="49" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B49" s="70"/>
+      <c r="B49" s="80"/>
       <c r="C49" s="22" t="s">
         <v>73</v>
       </c>
@@ -9852,7 +9852,7 @@
       <c r="S49" s="21"/>
       <c r="T49" s="21"/>
       <c r="U49" s="21"/>
-      <c r="V49" s="70"/>
+      <c r="V49" s="80"/>
       <c r="W49" s="22" t="s">
         <v>73</v>
       </c>
@@ -9957,7 +9957,7 @@
       <c r="AL50" s="30"/>
     </row>
     <row r="51" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B51" s="71" t="s">
+      <c r="B51" s="69" t="s">
         <v>74</v>
       </c>
       <c r="C51" s="45" t="s">
@@ -10026,7 +10026,7 @@
       <c r="S51" s="24"/>
       <c r="T51" s="24"/>
       <c r="U51" s="24"/>
-      <c r="V51" s="71" t="s">
+      <c r="V51" s="69" t="s">
         <v>74</v>
       </c>
       <c r="W51" s="45" t="s">
@@ -10094,7 +10094,7 @@
       </c>
     </row>
     <row r="52" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B52" s="72"/>
+      <c r="B52" s="70"/>
       <c r="C52" s="46" t="s">
         <v>76</v>
       </c>
@@ -10161,7 +10161,7 @@
       <c r="S52" s="12"/>
       <c r="T52" s="12"/>
       <c r="U52" s="12"/>
-      <c r="V52" s="72"/>
+      <c r="V52" s="70"/>
       <c r="W52" s="46" t="s">
         <v>76</v>
       </c>
@@ -10227,7 +10227,7 @@
       </c>
     </row>
     <row r="53" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B53" s="72"/>
+      <c r="B53" s="70"/>
       <c r="C53" s="46" t="s">
         <v>77</v>
       </c>
@@ -10294,7 +10294,7 @@
       <c r="S53" s="12"/>
       <c r="T53" s="12"/>
       <c r="U53" s="12"/>
-      <c r="V53" s="72"/>
+      <c r="V53" s="70"/>
       <c r="W53" s="46" t="s">
         <v>77</v>
       </c>
@@ -10360,7 +10360,7 @@
       </c>
     </row>
     <row r="54" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B54" s="72"/>
+      <c r="B54" s="70"/>
       <c r="C54" s="46" t="s">
         <v>78</v>
       </c>
@@ -10427,7 +10427,7 @@
       <c r="S54" s="12"/>
       <c r="T54" s="12"/>
       <c r="U54" s="12"/>
-      <c r="V54" s="72"/>
+      <c r="V54" s="70"/>
       <c r="W54" s="46" t="s">
         <v>78</v>
       </c>
@@ -10493,7 +10493,7 @@
       </c>
     </row>
     <row r="55" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B55" s="72"/>
+      <c r="B55" s="70"/>
       <c r="C55" s="46" t="s">
         <v>79</v>
       </c>
@@ -10560,7 +10560,7 @@
       <c r="S55" s="12"/>
       <c r="T55" s="12"/>
       <c r="U55" s="12"/>
-      <c r="V55" s="72"/>
+      <c r="V55" s="70"/>
       <c r="W55" s="46" t="s">
         <v>79</v>
       </c>
@@ -10626,7 +10626,7 @@
       </c>
     </row>
     <row r="56" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B56" s="72"/>
+      <c r="B56" s="70"/>
       <c r="C56" s="45" t="s">
         <v>80</v>
       </c>
@@ -10693,7 +10693,7 @@
       <c r="S56" s="12"/>
       <c r="T56" s="12"/>
       <c r="U56" s="12"/>
-      <c r="V56" s="72"/>
+      <c r="V56" s="70"/>
       <c r="W56" s="45" t="s">
         <v>80</v>
       </c>
@@ -10759,7 +10759,7 @@
       </c>
     </row>
     <row r="57" spans="2:38" x14ac:dyDescent="0.2">
-      <c r="B57" s="72"/>
+      <c r="B57" s="70"/>
       <c r="C57" s="47" t="s">
         <v>87</v>
       </c>
@@ -10826,7 +10826,7 @@
       <c r="S57" s="13"/>
       <c r="T57" s="13"/>
       <c r="U57" s="13"/>
-      <c r="V57" s="72"/>
+      <c r="V57" s="70"/>
       <c r="W57" s="47" t="s">
         <v>87</v>
       </c>
@@ -10978,6 +10978,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="V44:V49"/>
+    <mergeCell ref="V51:V57"/>
+    <mergeCell ref="X4:AA4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="AE4:AH4"/>
+    <mergeCell ref="V28:V35"/>
+    <mergeCell ref="V37:V39"/>
+    <mergeCell ref="V40:V42"/>
+    <mergeCell ref="AI4:AL4"/>
+    <mergeCell ref="V4:W5"/>
+    <mergeCell ref="V6:V10"/>
+    <mergeCell ref="V12:V19"/>
+    <mergeCell ref="V21:V26"/>
     <mergeCell ref="B51:B57"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="H4:J4"/>
@@ -10994,19 +11007,6 @@
     <mergeCell ref="B12:B19"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="B37:B39"/>
-    <mergeCell ref="AI4:AL4"/>
-    <mergeCell ref="V4:W5"/>
-    <mergeCell ref="V6:V10"/>
-    <mergeCell ref="V12:V19"/>
-    <mergeCell ref="V21:V26"/>
-    <mergeCell ref="V44:V49"/>
-    <mergeCell ref="V51:V57"/>
-    <mergeCell ref="X4:AA4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="AE4:AH4"/>
-    <mergeCell ref="V28:V35"/>
-    <mergeCell ref="V37:V39"/>
-    <mergeCell ref="V40:V42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11020,7 +11020,7 @@
   <dimension ref="A1:AE118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+      <selection activeCell="U61" sqref="B4:U61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.55" x14ac:dyDescent="0.2"/>
@@ -11099,40 +11099,40 @@
       </c>
     </row>
     <row r="4" spans="2:25" ht="15.05" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="73" t="s">
+      <c r="C4" s="87"/>
+      <c r="D4" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
       <c r="H4" s="59"/>
-      <c r="I4" s="73" t="s">
+      <c r="I4" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
       <c r="L4" s="59"/>
-      <c r="M4" s="73" t="s">
+      <c r="M4" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="71"/>
       <c r="Q4" s="59"/>
-      <c r="R4" s="73" t="s">
+      <c r="R4" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="71"/>
     </row>
     <row r="5" spans="2:25" ht="54.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
       <c r="D5" s="5" t="s">
         <v>53</v>
       </c>
@@ -11183,45 +11183,45 @@
       </c>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B6" s="80" t="s">
-        <v>100</v>
+      <c r="B6" s="72" t="s">
+        <v>98</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="88">
+      <c r="D6" s="75">
         <f>1150/81</f>
         <v>14.197530864197532</v>
       </c>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="88">
+      <c r="I6" s="75">
         <f>1150/81</f>
         <v>14.197530864197532</v>
       </c>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="88">
+      <c r="M6" s="75">
         <f>1150/81</f>
         <v>14.197530864197532</v>
       </c>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88"/>
-      <c r="P6" s="88"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="75"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="88">
+      <c r="R6" s="75">
         <f>500/81</f>
         <v>6.1728395061728394</v>
       </c>
-      <c r="S6" s="88"/>
-      <c r="T6" s="88"/>
-      <c r="U6" s="88"/>
+      <c r="S6" s="75"/>
+      <c r="T6" s="75"/>
+      <c r="U6" s="75"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B7" s="81"/>
+      <c r="B7" s="73"/>
       <c r="C7" s="62" t="s">
         <v>70</v>
       </c>
@@ -11290,7 +11290,7 @@
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B8" s="81"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="8" t="s">
         <v>59</v>
       </c>
@@ -11359,7 +11359,7 @@
       </c>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B9" s="81"/>
+      <c r="B9" s="73"/>
       <c r="C9" s="8" t="s">
         <v>60</v>
       </c>
@@ -11428,7 +11428,7 @@
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B10" s="81"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="8" t="s">
         <v>61</v>
       </c>
@@ -11500,7 +11500,7 @@
       <c r="Y10" s="34"/>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B11" s="82"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="15" t="s">
         <v>23</v>
       </c>
@@ -11591,7 +11591,7 @@
       <c r="U12" s="30"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="81" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="36" t="s">
@@ -11662,7 +11662,7 @@
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B14" s="84"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="36" t="s">
         <v>64</v>
       </c>
@@ -11731,7 +11731,7 @@
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B15" s="84"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="37" t="s">
         <v>28</v>
       </c>
@@ -11800,7 +11800,7 @@
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B16" s="84"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="37" t="s">
         <v>65</v>
       </c>
@@ -11869,7 +11869,7 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B17" s="84"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="37" t="s">
         <v>30</v>
       </c>
@@ -11941,7 +11941,7 @@
       <c r="Y17" s="65"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B18" s="84"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="37" t="s">
         <v>31</v>
       </c>
@@ -12010,7 +12010,7 @@
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B19" s="84"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="37" t="s">
         <v>32</v>
       </c>
@@ -12079,7 +12079,7 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B20" s="85"/>
+      <c r="B20" s="83"/>
       <c r="C20" s="36" t="s">
         <v>26</v>
       </c>
@@ -12291,7 +12291,7 @@
       </c>
     </row>
     <row r="23" spans="1:25" ht="12.55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="86"/>
+      <c r="B23" s="76"/>
       <c r="C23" s="38" t="s">
         <v>64</v>
       </c>
@@ -12363,7 +12363,7 @@
       <c r="Y23" s="65"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B24" s="86"/>
+      <c r="B24" s="76"/>
       <c r="C24" s="39" t="s">
         <v>28</v>
       </c>
@@ -12432,7 +12432,7 @@
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B25" s="86"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="39" t="s">
         <v>65</v>
       </c>
@@ -12501,7 +12501,7 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B26" s="86"/>
+      <c r="B26" s="76"/>
       <c r="C26" s="39" t="s">
         <v>66</v>
       </c>
@@ -12570,7 +12570,7 @@
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B27" s="86"/>
+      <c r="B27" s="76"/>
       <c r="C27" s="39" t="s">
         <v>34</v>
       </c>
@@ -12730,8 +12730,8 @@
       <c r="U29" s="30"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B30" s="74" t="s">
-        <v>99</v>
+      <c r="B30" s="78" t="s">
+        <v>97</v>
       </c>
       <c r="C30" s="19" t="s">
         <v>37</v>
@@ -12801,7 +12801,7 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B31" s="74"/>
+      <c r="B31" s="78"/>
       <c r="C31" s="19" t="s">
         <v>44</v>
       </c>
@@ -12870,7 +12870,7 @@
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B32" s="74"/>
+      <c r="B32" s="78"/>
       <c r="C32" s="19" t="s">
         <v>45</v>
       </c>
@@ -12939,7 +12939,7 @@
       </c>
     </row>
     <row r="33" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B33" s="74"/>
+      <c r="B33" s="78"/>
       <c r="C33" s="19" t="s">
         <v>69</v>
       </c>
@@ -13008,9 +13008,9 @@
       </c>
     </row>
     <row r="34" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B34" s="74"/>
+      <c r="B34" s="78"/>
       <c r="C34" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D34" s="20">
         <f>D35+D38</f>
@@ -13077,7 +13077,7 @@
       </c>
     </row>
     <row r="35" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B35" s="74"/>
+      <c r="B35" s="78"/>
       <c r="C35" s="19" t="s">
         <v>47</v>
       </c>
@@ -13147,7 +13147,7 @@
       <c r="W35" s="65"/>
     </row>
     <row r="36" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B36" s="74"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="19" t="s">
         <v>40</v>
       </c>
@@ -13216,7 +13216,7 @@
       </c>
     </row>
     <row r="37" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B37" s="74"/>
+      <c r="B37" s="78"/>
       <c r="C37" s="19" t="s">
         <v>41</v>
       </c>
@@ -13285,9 +13285,9 @@
       </c>
     </row>
     <row r="38" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B38" s="74"/>
+      <c r="B38" s="78"/>
       <c r="C38" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38" s="20">
         <f>MainTab_connection!E20</f>
@@ -13450,7 +13450,7 @@
     <row r="41" spans="2:31" ht="15.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="93"/>
       <c r="C41" s="41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D41" s="27">
         <f>-MainTab_connection!E25</f>
@@ -13588,7 +13588,7 @@
     </row>
     <row r="43" spans="2:31" ht="15.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="92" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C43" s="40" t="s">
         <v>47</v>
@@ -13668,7 +13668,7 @@
     <row r="44" spans="2:31" ht="15.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="93"/>
       <c r="C44" s="41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D44" s="27">
         <f>D41/D38*1000</f>
@@ -13826,8 +13826,8 @@
       <c r="U46" s="32"/>
     </row>
     <row r="47" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B47" s="69" t="s">
-        <v>96</v>
+      <c r="B47" s="79" t="s">
+        <v>99</v>
       </c>
       <c r="C47" s="44" t="s">
         <v>70</v>
@@ -13897,9 +13897,9 @@
       </c>
     </row>
     <row r="48" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B48" s="70"/>
+      <c r="B48" s="80"/>
       <c r="C48" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D48" s="21">
         <f>(D9+D11)/(D30+D35)*1000</f>
@@ -13966,7 +13966,7 @@
       </c>
     </row>
     <row r="49" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B49" s="70"/>
+      <c r="B49" s="80"/>
       <c r="C49" s="22" t="s">
         <v>59</v>
       </c>
@@ -14035,7 +14035,7 @@
       </c>
     </row>
     <row r="50" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B50" s="70"/>
+      <c r="B50" s="80"/>
       <c r="C50" s="23" t="s">
         <v>60</v>
       </c>
@@ -14105,7 +14105,7 @@
       <c r="W50" s="63"/>
     </row>
     <row r="51" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B51" s="70"/>
+      <c r="B51" s="80"/>
       <c r="C51" s="23" t="s">
         <v>71</v>
       </c>
@@ -14175,7 +14175,7 @@
       <c r="W51" s="63"/>
     </row>
     <row r="52" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B52" s="70"/>
+      <c r="B52" s="80"/>
       <c r="C52" s="22" t="s">
         <v>72</v>
       </c>
@@ -14244,9 +14244,9 @@
       </c>
     </row>
     <row r="53" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B53" s="70"/>
+      <c r="B53" s="80"/>
       <c r="C53" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D53" s="21">
         <f>D11/(D35+D38)*1000</f>
@@ -14335,7 +14335,7 @@
       <c r="U54" s="30"/>
     </row>
     <row r="55" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B55" s="71" t="s">
+      <c r="B55" s="69" t="s">
         <v>74</v>
       </c>
       <c r="C55" s="60" t="s">
@@ -14407,7 +14407,7 @@
       <c r="W55" s="63"/>
     </row>
     <row r="56" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B56" s="72"/>
+      <c r="B56" s="70"/>
       <c r="C56" s="45" t="s">
         <v>76</v>
       </c>
@@ -14476,7 +14476,7 @@
       </c>
     </row>
     <row r="57" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B57" s="72"/>
+      <c r="B57" s="70"/>
       <c r="C57" s="45" t="s">
         <v>77</v>
       </c>
@@ -14548,7 +14548,7 @@
       <c r="Y57" s="68"/>
     </row>
     <row r="58" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B58" s="72"/>
+      <c r="B58" s="70"/>
       <c r="C58" s="45" t="s">
         <v>78</v>
       </c>
@@ -14620,7 +14620,7 @@
       <c r="Y58" s="49"/>
     </row>
     <row r="59" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B59" s="72"/>
+      <c r="B59" s="70"/>
       <c r="C59" s="45" t="s">
         <v>79</v>
       </c>
@@ -14689,7 +14689,7 @@
       </c>
     </row>
     <row r="60" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B60" s="72"/>
+      <c r="B60" s="70"/>
       <c r="C60" s="45" t="s">
         <v>80</v>
       </c>
@@ -14908,40 +14908,40 @@
       <c r="U65" s="1"/>
     </row>
     <row r="66" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B66" s="78" t="s">
+      <c r="B66" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="C66" s="78"/>
-      <c r="D66" s="73" t="s">
+      <c r="C66" s="87"/>
+      <c r="D66" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="E66" s="73"/>
-      <c r="F66" s="73"/>
-      <c r="G66" s="73"/>
+      <c r="E66" s="71"/>
+      <c r="F66" s="71"/>
+      <c r="G66" s="71"/>
       <c r="H66" s="59"/>
-      <c r="I66" s="73" t="s">
+      <c r="I66" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="J66" s="73"/>
-      <c r="K66" s="73"/>
+      <c r="J66" s="71"/>
+      <c r="K66" s="71"/>
       <c r="L66" s="59"/>
-      <c r="M66" s="73" t="s">
+      <c r="M66" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="N66" s="73"/>
-      <c r="O66" s="73"/>
-      <c r="P66" s="73"/>
+      <c r="N66" s="71"/>
+      <c r="O66" s="71"/>
+      <c r="P66" s="71"/>
       <c r="Q66" s="59"/>
-      <c r="R66" s="73" t="s">
+      <c r="R66" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="S66" s="73"/>
-      <c r="T66" s="73"/>
-      <c r="U66" s="73"/>
+      <c r="S66" s="71"/>
+      <c r="T66" s="71"/>
+      <c r="U66" s="71"/>
     </row>
     <row r="67" spans="2:25" ht="54.5" x14ac:dyDescent="0.2">
-      <c r="B67" s="79"/>
-      <c r="C67" s="79"/>
+      <c r="B67" s="88"/>
+      <c r="C67" s="88"/>
       <c r="D67" s="5" t="s">
         <v>53</v>
       </c>
@@ -14992,7 +14992,7 @@
       </c>
     </row>
     <row r="68" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B68" s="81"/>
+      <c r="B68" s="73"/>
       <c r="C68" s="8" t="s">
         <v>59</v>
       </c>
@@ -15061,7 +15061,7 @@
       </c>
     </row>
     <row r="69" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B69" s="81"/>
+      <c r="B69" s="73"/>
       <c r="C69" s="8" t="s">
         <v>60</v>
       </c>
@@ -15130,7 +15130,7 @@
       </c>
     </row>
     <row r="70" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B70" s="81"/>
+      <c r="B70" s="73"/>
       <c r="C70" s="8" t="s">
         <v>61</v>
       </c>
@@ -15199,7 +15199,7 @@
       </c>
     </row>
     <row r="71" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B71" s="82"/>
+      <c r="B71" s="74"/>
       <c r="C71" s="15" t="s">
         <v>23</v>
       </c>
@@ -15290,7 +15290,7 @@
       <c r="U72" s="30"/>
     </row>
     <row r="73" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B73" s="83" t="s">
+      <c r="B73" s="81" t="s">
         <v>63</v>
       </c>
       <c r="C73" s="36" t="s">
@@ -15361,7 +15361,7 @@
       </c>
     </row>
     <row r="74" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B74" s="84"/>
+      <c r="B74" s="82"/>
       <c r="C74" s="36" t="s">
         <v>64</v>
       </c>
@@ -15430,7 +15430,7 @@
       </c>
     </row>
     <row r="75" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B75" s="84"/>
+      <c r="B75" s="82"/>
       <c r="C75" s="37" t="s">
         <v>28</v>
       </c>
@@ -15499,7 +15499,7 @@
       </c>
     </row>
     <row r="76" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B76" s="84"/>
+      <c r="B76" s="82"/>
       <c r="C76" s="37" t="s">
         <v>65</v>
       </c>
@@ -15568,7 +15568,7 @@
       </c>
     </row>
     <row r="77" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B77" s="84"/>
+      <c r="B77" s="82"/>
       <c r="C77" s="37" t="s">
         <v>30</v>
       </c>
@@ -15640,7 +15640,7 @@
       <c r="Y77" s="65"/>
     </row>
     <row r="78" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B78" s="84"/>
+      <c r="B78" s="82"/>
       <c r="C78" s="37" t="s">
         <v>31</v>
       </c>
@@ -15709,7 +15709,7 @@
       </c>
     </row>
     <row r="79" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B79" s="84"/>
+      <c r="B79" s="82"/>
       <c r="C79" s="37" t="s">
         <v>32</v>
       </c>
@@ -15778,7 +15778,7 @@
       </c>
     </row>
     <row r="80" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B80" s="85"/>
+      <c r="B80" s="83"/>
       <c r="C80" s="36" t="s">
         <v>26</v>
       </c>
@@ -15869,7 +15869,7 @@
       <c r="U81" s="30"/>
     </row>
     <row r="82" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B82" s="86" t="s">
+      <c r="B82" s="76" t="s">
         <v>83</v>
       </c>
       <c r="C82" s="38" t="s">
@@ -15940,7 +15940,7 @@
       </c>
     </row>
     <row r="83" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B83" s="87"/>
+      <c r="B83" s="77"/>
       <c r="C83" s="39" t="s">
         <v>28</v>
       </c>
@@ -16009,7 +16009,7 @@
       </c>
     </row>
     <row r="84" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B84" s="87"/>
+      <c r="B84" s="77"/>
       <c r="C84" s="39" t="s">
         <v>65</v>
       </c>
@@ -16078,7 +16078,7 @@
       </c>
     </row>
     <row r="85" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B85" s="87"/>
+      <c r="B85" s="77"/>
       <c r="C85" s="39" t="s">
         <v>66</v>
       </c>
@@ -16147,7 +16147,7 @@
       </c>
     </row>
     <row r="86" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B86" s="87"/>
+      <c r="B86" s="77"/>
       <c r="C86" s="39" t="s">
         <v>34</v>
       </c>
@@ -16216,7 +16216,7 @@
       </c>
     </row>
     <row r="87" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B87" s="86"/>
+      <c r="B87" s="76"/>
       <c r="C87" s="38" t="s">
         <v>67</v>
       </c>
@@ -16307,8 +16307,8 @@
       <c r="U88" s="30"/>
     </row>
     <row r="89" spans="2:21" ht="12.55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="74" t="s">
-        <v>91</v>
+      <c r="B89" s="78" t="s">
+        <v>97</v>
       </c>
       <c r="C89" s="19" t="s">
         <v>37</v>
@@ -16378,7 +16378,7 @@
       </c>
     </row>
     <row r="90" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B90" s="74"/>
+      <c r="B90" s="78"/>
       <c r="C90" s="19" t="s">
         <v>44</v>
       </c>
@@ -16447,7 +16447,7 @@
       </c>
     </row>
     <row r="91" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B91" s="74"/>
+      <c r="B91" s="78"/>
       <c r="C91" s="19" t="s">
         <v>45</v>
       </c>
@@ -16516,7 +16516,7 @@
       </c>
     </row>
     <row r="92" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B92" s="74"/>
+      <c r="B92" s="78"/>
       <c r="C92" s="19" t="s">
         <v>69</v>
       </c>
@@ -16585,7 +16585,7 @@
       </c>
     </row>
     <row r="93" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B93" s="74"/>
+      <c r="B93" s="78"/>
       <c r="C93" s="19" t="s">
         <v>47</v>
       </c>
@@ -16654,7 +16654,7 @@
       </c>
     </row>
     <row r="94" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B94" s="74"/>
+      <c r="B94" s="78"/>
       <c r="C94" s="19" t="s">
         <v>40</v>
       </c>
@@ -16723,7 +16723,7 @@
       </c>
     </row>
     <row r="95" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B95" s="74"/>
+      <c r="B95" s="78"/>
       <c r="C95" s="19" t="s">
         <v>41</v>
       </c>
@@ -16792,9 +16792,9 @@
       </c>
     </row>
     <row r="96" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B96" s="74"/>
+      <c r="B96" s="78"/>
       <c r="C96" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D96" s="20">
         <f>MainTab_connection!T20</f>
@@ -16956,7 +16956,7 @@
     <row r="99" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B99" s="93"/>
       <c r="C99" s="41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D99" s="27">
         <f>-MainTab_connection!T25</f>
@@ -17093,7 +17093,7 @@
     </row>
     <row r="101" spans="2:24" ht="12.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="92" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C101" s="40" t="s">
         <v>47</v>
@@ -17166,7 +17166,7 @@
     <row r="102" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B102" s="93"/>
       <c r="C102" s="41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D102" s="58">
         <f t="shared" ref="D102:R102" si="44">D99/D96*1000</f>
@@ -17324,8 +17324,8 @@
       <c r="U104" s="32"/>
     </row>
     <row r="105" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B105" s="69" t="s">
-        <v>85</v>
+      <c r="B105" s="79" t="s">
+        <v>100</v>
       </c>
       <c r="C105" s="44" t="s">
         <v>70</v>
@@ -17395,7 +17395,7 @@
       </c>
     </row>
     <row r="106" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B106" s="70"/>
+      <c r="B106" s="80"/>
       <c r="C106" s="22" t="s">
         <v>59</v>
       </c>
@@ -17464,7 +17464,7 @@
       </c>
     </row>
     <row r="107" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B107" s="70"/>
+      <c r="B107" s="80"/>
       <c r="C107" s="23" t="s">
         <v>60</v>
       </c>
@@ -17534,7 +17534,7 @@
       <c r="W107" s="63"/>
     </row>
     <row r="108" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B108" s="70"/>
+      <c r="B108" s="80"/>
       <c r="C108" s="23" t="s">
         <v>71</v>
       </c>
@@ -17604,7 +17604,7 @@
       <c r="W108" s="63"/>
     </row>
     <row r="109" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B109" s="70"/>
+      <c r="B109" s="80"/>
       <c r="C109" s="22" t="s">
         <v>72</v>
       </c>
@@ -17673,9 +17673,9 @@
       </c>
     </row>
     <row r="110" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B110" s="70"/>
+      <c r="B110" s="80"/>
       <c r="C110" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D110" s="56">
         <f t="shared" ref="D110:U110" si="53">D71/(D93+D96)*1000</f>
@@ -17764,7 +17764,7 @@
       <c r="U111" s="30"/>
     </row>
     <row r="112" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B112" s="71" t="s">
+      <c r="B112" s="69" t="s">
         <v>74</v>
       </c>
       <c r="C112" s="60" t="s">
@@ -17836,7 +17836,7 @@
       <c r="W112" s="63"/>
     </row>
     <row r="113" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B113" s="72"/>
+      <c r="B113" s="70"/>
       <c r="C113" s="45" t="s">
         <v>76</v>
       </c>
@@ -17905,7 +17905,7 @@
       </c>
     </row>
     <row r="114" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B114" s="72"/>
+      <c r="B114" s="70"/>
       <c r="C114" s="45" t="s">
         <v>77</v>
       </c>
@@ -17974,7 +17974,7 @@
       </c>
     </row>
     <row r="115" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B115" s="72"/>
+      <c r="B115" s="70"/>
       <c r="C115" s="45" t="s">
         <v>78</v>
       </c>
@@ -18043,7 +18043,7 @@
       </c>
     </row>
     <row r="116" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B116" s="72"/>
+      <c r="B116" s="70"/>
       <c r="C116" s="45" t="s">
         <v>79</v>
       </c>
@@ -18112,7 +18112,7 @@
       </c>
     </row>
     <row r="117" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B117" s="72"/>
+      <c r="B117" s="70"/>
       <c r="C117" s="45" t="s">
         <v>80</v>
       </c>
@@ -18253,6 +18253,21 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B112:B118"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="B47:B53"/>
+    <mergeCell ref="B105:B110"/>
+    <mergeCell ref="B13:B20"/>
+    <mergeCell ref="B73:B80"/>
+    <mergeCell ref="B82:B87"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="B89:B96"/>
+    <mergeCell ref="B68:B71"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="I4:K4"/>
     <mergeCell ref="M4:P4"/>
@@ -18268,21 +18283,6 @@
     <mergeCell ref="M6:P6"/>
     <mergeCell ref="R6:U6"/>
     <mergeCell ref="B55:B61"/>
-    <mergeCell ref="B112:B118"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="B47:B53"/>
-    <mergeCell ref="B105:B110"/>
-    <mergeCell ref="B13:B20"/>
-    <mergeCell ref="B73:B80"/>
-    <mergeCell ref="B82:B87"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="B89:B96"/>
-    <mergeCell ref="B68:B71"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>